<commit_message>
created script to calc pH TRIS
</commit_message>
<xml_diff>
--- a/airica/data/Aug_20_Wadden_sea_B1_AIRICA.xlsx
+++ b/airica/data/Aug_20_Wadden_sea_B1_AIRICA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_LAB/Aug_20_Wadden_sea_B1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/lab-work/airica/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{2ADD0B49-2137-472B-837C-A2FF8AF723D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D658E6C5-047E-4854-B5B3-EE23AEC3D65E}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{2ADD0B49-2137-472B-837C-A2FF8AF723D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1C3E569-C401-4ABB-8CA5-A307A83500BC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D1C24D6-B482-4633-80E7-FE6A1A2CCD8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="108">
   <si>
     <t>all to stripper</t>
   </si>
@@ -165,9 +165,6 @@
     <t>area2</t>
   </si>
   <si>
-    <t>are3</t>
-  </si>
-  <si>
     <t>area4</t>
   </si>
   <si>
@@ -265,6 +262,102 @@
   </si>
   <si>
     <t>0-0 0 (0)B120.dat</t>
+  </si>
+  <si>
+    <t>area3</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>CRM1</t>
+  </si>
+  <si>
+    <t>CRM2</t>
+  </si>
+  <si>
+    <t>CRM3</t>
+  </si>
+  <si>
+    <t>CRM4</t>
+  </si>
+  <si>
+    <t>CRM5</t>
+  </si>
+  <si>
+    <t>CRM6</t>
+  </si>
+  <si>
+    <t>CRM7</t>
+  </si>
+  <si>
+    <t>CRM8</t>
+  </si>
+  <si>
+    <t>CRM9</t>
+  </si>
+  <si>
+    <t>CRM10</t>
+  </si>
+  <si>
+    <t>CRM11</t>
+  </si>
+  <si>
+    <t>CRM12</t>
+  </si>
+  <si>
+    <t>CRM13</t>
+  </si>
+  <si>
+    <t>B127</t>
+  </si>
+  <si>
+    <t>B125</t>
+  </si>
+  <si>
+    <t>B122</t>
+  </si>
+  <si>
+    <t>B124</t>
+  </si>
+  <si>
+    <t>B129</t>
+  </si>
+  <si>
+    <t>B129_2</t>
+  </si>
+  <si>
+    <t>B123</t>
+  </si>
+  <si>
+    <t>B128</t>
+  </si>
+  <si>
+    <t>B121</t>
+  </si>
+  <si>
+    <t>B117</t>
+  </si>
+  <si>
+    <t>B126</t>
+  </si>
+  <si>
+    <t>B119</t>
+  </si>
+  <si>
+    <t>B120</t>
+  </si>
+  <si>
+    <t>B116</t>
+  </si>
+  <si>
+    <t>B118</t>
+  </si>
+  <si>
+    <t>B130</t>
   </si>
 </sst>
 </file>
@@ -648,35 +741,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E656E55-4C50-4FC5-BBD3-EE98058A854C}">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="L43:M43"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="15.26953125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="2"/>
-    <col min="6" max="6" width="23.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.90625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.7265625" style="2" customWidth="1"/>
-    <col min="13" max="17" width="8.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.7265625" style="2"/>
-    <col min="19" max="19" width="10.81640625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="22" style="2" customWidth="1"/>
-    <col min="21" max="25" width="8.7265625" style="2"/>
-    <col min="26" max="26" width="8.7265625" style="4"/>
-    <col min="27" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.7109375" style="2"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="2" customWidth="1"/>
+    <col min="14" max="18" width="8.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" style="2"/>
+    <col min="20" max="20" width="10.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="22" style="2" customWidth="1"/>
+    <col min="22" max="26" width="8.7109375" style="2"/>
+    <col min="27" max="27" width="8.7109375" style="4"/>
+    <col min="28" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -693,70 +786,73 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="T1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -772,8 +868,8 @@
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>30</v>
+      <c r="F2" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>30</v>
@@ -785,13 +881,13 @@
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>32</v>
@@ -800,20 +896,23 @@
         <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="5"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA2" s="5"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -829,57 +928,60 @@
       <c r="E3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2">
         <v>400</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>60</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>120</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
         <v>1500</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>1000</v>
       </c>
-      <c r="L3" s="2">
-        <v>150</v>
-      </c>
       <c r="M3" s="2">
         <v>150</v>
       </c>
-      <c r="N3" s="1">
-        <f>J3/100</f>
+      <c r="N3" s="2">
+        <v>150</v>
+      </c>
+      <c r="O3" s="1">
+        <f>K3/100</f>
         <v>15</v>
       </c>
-      <c r="O3" s="2">
-        <v>3</v>
-      </c>
       <c r="P3" s="2">
         <v>3</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>0</v>
+      <c r="Q3" s="2">
+        <v>3</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -895,57 +997,60 @@
       <c r="E4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2">
         <v>400</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>60</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>120</v>
       </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
         <v>1700</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>1000</v>
       </c>
-      <c r="L4" s="2">
-        <v>150</v>
-      </c>
       <c r="M4" s="2">
         <v>150</v>
       </c>
-      <c r="N4" s="1">
-        <f t="shared" ref="N4:N20" si="0">J4/100</f>
+      <c r="N4" s="2">
+        <v>150</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O20" si="0">K4/100</f>
         <v>17</v>
       </c>
-      <c r="O4" s="2">
-        <v>3</v>
-      </c>
       <c r="P4" s="2">
         <v>3</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>0</v>
+      <c r="Q4" s="2">
+        <v>3</v>
       </c>
       <c r="R4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -961,57 +1066,60 @@
       <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="2">
         <v>400</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>60</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>120</v>
       </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
         <v>1700</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>1000</v>
       </c>
-      <c r="L5" s="2">
-        <v>150</v>
-      </c>
       <c r="M5" s="2">
         <v>150</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="2">
+        <v>150</v>
+      </c>
+      <c r="O5" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O5" s="2">
-        <v>3</v>
-      </c>
       <c r="P5" s="2">
         <v>3</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>0</v>
+      <c r="Q5" s="2">
+        <v>3</v>
       </c>
       <c r="R5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1027,57 +1135,60 @@
       <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="2">
         <v>400</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>60</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>120</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
         <v>1800</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>1000</v>
       </c>
-      <c r="L6" s="2">
-        <v>150</v>
-      </c>
       <c r="M6" s="2">
         <v>150</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="2">
+        <v>150</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O6" s="2">
-        <v>3</v>
-      </c>
       <c r="P6" s="2">
         <v>3</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>0</v>
+      <c r="Q6" s="2">
+        <v>3</v>
       </c>
       <c r="R6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T6" s="4" t="s">
+      <c r="T6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1093,57 +1204,60 @@
       <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="2">
         <v>400</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>60</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>120</v>
       </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
         <v>1900</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>1000</v>
       </c>
-      <c r="L7" s="2">
-        <v>150</v>
-      </c>
       <c r="M7" s="2">
         <v>150</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="2">
+        <v>150</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="O7" s="2">
-        <v>3</v>
-      </c>
       <c r="P7" s="2">
         <v>3</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>0</v>
+      <c r="Q7" s="2">
+        <v>3</v>
       </c>
       <c r="R7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="4" t="s">
+      <c r="T7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -1159,59 +1273,62 @@
       <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="2">
         <v>400</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>60</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>120</v>
       </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>2200</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>1000</v>
       </c>
-      <c r="L8" s="2">
-        <v>150</v>
-      </c>
       <c r="M8" s="2">
         <v>150</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="2">
+        <v>150</v>
+      </c>
+      <c r="O8" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="O8" s="2">
-        <v>3</v>
-      </c>
       <c r="P8" s="2">
         <v>3</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>0</v>
+      <c r="Q8" s="2">
+        <v>3</v>
       </c>
       <c r="R8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="U8" s="2">
+      <c r="T8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>38</v>
@@ -1220,64 +1337,67 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2">
         <v>27</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="2">
         <v>400</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>60</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>120</v>
       </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <v>1800</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>1000</v>
       </c>
-      <c r="L9" s="2">
-        <v>150</v>
-      </c>
       <c r="M9" s="2">
         <v>150</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="2">
+        <v>150</v>
+      </c>
+      <c r="O9" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O9" s="2">
-        <v>3</v>
-      </c>
       <c r="P9" s="2">
         <v>3</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>0</v>
+      <c r="Q9" s="2">
+        <v>3</v>
       </c>
       <c r="R9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="U9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>38</v>
@@ -1286,64 +1406,67 @@
         <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2">
         <v>25</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="2">
         <v>400</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>60</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>120</v>
       </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
         <v>1800</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>1000</v>
       </c>
-      <c r="L10" s="2">
-        <v>150</v>
-      </c>
       <c r="M10" s="2">
         <v>150</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="2">
+        <v>150</v>
+      </c>
+      <c r="O10" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O10" s="2">
-        <v>3</v>
-      </c>
       <c r="P10" s="2">
         <v>3</v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>0</v>
+      <c r="Q10" s="2">
+        <v>3</v>
       </c>
       <c r="R10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U10" s="2">
+      <c r="T10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V10" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
@@ -1352,64 +1475,67 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2">
         <v>22</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="2">
         <v>400</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>60</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>120</v>
       </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
         <v>1800</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>1000</v>
       </c>
-      <c r="L11" s="2">
-        <v>150</v>
-      </c>
       <c r="M11" s="2">
         <v>150</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="2">
+        <v>150</v>
+      </c>
+      <c r="O11" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O11" s="2">
-        <v>3</v>
-      </c>
       <c r="P11" s="2">
         <v>3</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>0</v>
+      <c r="Q11" s="2">
+        <v>3</v>
       </c>
       <c r="R11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="U11" s="2">
+      <c r="T11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="V11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>38</v>
@@ -1418,64 +1544,67 @@
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2">
         <v>24</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="2">
         <v>400</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>60</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>120</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
         <v>1800</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>1000</v>
       </c>
-      <c r="L12" s="2">
-        <v>150</v>
-      </c>
       <c r="M12" s="2">
         <v>150</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="2">
+        <v>150</v>
+      </c>
+      <c r="O12" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O12" s="2">
-        <v>3</v>
-      </c>
       <c r="P12" s="2">
         <v>3</v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>0</v>
+      <c r="Q12" s="2">
+        <v>3</v>
       </c>
       <c r="R12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="U12" s="2">
+      <c r="T12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>38</v>
@@ -1484,67 +1613,70 @@
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2">
         <v>29</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="2">
         <v>400</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>60</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>120</v>
       </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
         <v>1800</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>1000</v>
       </c>
-      <c r="L13" s="2">
-        <v>150</v>
-      </c>
       <c r="M13" s="2">
         <v>150</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="2">
+        <v>150</v>
+      </c>
+      <c r="O13" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O13" s="2">
-        <v>3</v>
-      </c>
       <c r="P13" s="2">
         <v>3</v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>0</v>
+      <c r="Q13" s="2">
+        <v>3</v>
       </c>
       <c r="R13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="U13" s="2">
-        <v>4</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="T13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V13" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>38</v>
@@ -1553,67 +1685,70 @@
         <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="2">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="2">
         <v>400</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>60</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>120</v>
       </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
         <v>1800</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>1000</v>
       </c>
-      <c r="L14" s="2">
-        <v>150</v>
-      </c>
       <c r="M14" s="2">
         <v>150</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="2">
+        <v>150</v>
+      </c>
+      <c r="O14" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O14" s="2">
-        <v>3</v>
-      </c>
       <c r="P14" s="2">
         <v>3</v>
       </c>
-      <c r="Q14" s="2" t="s">
-        <v>0</v>
+      <c r="Q14" s="2">
+        <v>3</v>
       </c>
       <c r="R14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="U14" s="2">
+      <c r="T14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>39</v>
@@ -1624,65 +1759,68 @@
       <c r="E15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="2">
         <v>400</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>60</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>120</v>
       </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <v>1400</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>1000</v>
       </c>
-      <c r="L15" s="2">
-        <v>150</v>
-      </c>
       <c r="M15" s="2">
         <v>150</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="2">
+        <v>150</v>
+      </c>
+      <c r="O15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="O15" s="2">
-        <v>3</v>
-      </c>
       <c r="P15" s="2">
         <v>3</v>
       </c>
-      <c r="Q15" s="2" t="s">
-        <v>0</v>
+      <c r="Q15" s="2">
+        <v>3</v>
       </c>
       <c r="R15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="V15" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="U15" s="2">
-        <v>4</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>39</v>
@@ -1693,65 +1831,68 @@
       <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="2">
         <v>400</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>60</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>120</v>
       </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
         <v>1500</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>1000</v>
       </c>
-      <c r="L16" s="2">
-        <v>150</v>
-      </c>
       <c r="M16" s="2">
         <v>150</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="2">
+        <v>150</v>
+      </c>
+      <c r="O16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="O16" s="2">
-        <v>3</v>
-      </c>
       <c r="P16" s="2">
         <v>3</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>0</v>
+      <c r="Q16" s="2">
+        <v>3</v>
       </c>
       <c r="R16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="U16" s="2">
+      <c r="T16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V16" s="2">
         <v>2</v>
       </c>
-      <c r="Z16" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AA16" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
@@ -1762,62 +1903,65 @@
       <c r="E17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="2">
         <v>400</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>60</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>120</v>
       </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
         <v>1700</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>1000</v>
       </c>
-      <c r="L17" s="2">
-        <v>150</v>
-      </c>
       <c r="M17" s="2">
         <v>150</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="2">
+        <v>150</v>
+      </c>
+      <c r="O17" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O17" s="2">
-        <v>3</v>
-      </c>
       <c r="P17" s="2">
         <v>3</v>
       </c>
-      <c r="Q17" s="2" t="s">
-        <v>0</v>
+      <c r="Q17" s="2">
+        <v>3</v>
       </c>
       <c r="R17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="U17" s="2">
+      <c r="T17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>39</v>
@@ -1828,62 +1972,65 @@
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="2">
         <v>400</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>60</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>120</v>
       </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
         <v>1800</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>1000</v>
       </c>
-      <c r="L18" s="2">
-        <v>150</v>
-      </c>
       <c r="M18" s="2">
         <v>150</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="2">
+        <v>150</v>
+      </c>
+      <c r="O18" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O18" s="2">
-        <v>3</v>
-      </c>
       <c r="P18" s="2">
         <v>3</v>
       </c>
-      <c r="Q18" s="2" t="s">
-        <v>0</v>
+      <c r="Q18" s="2">
+        <v>3</v>
       </c>
       <c r="R18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="U18" s="2">
+      <c r="T18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>39</v>
@@ -1894,62 +2041,65 @@
       <c r="E19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="2">
         <v>400</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>60</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>120</v>
       </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
         <v>1900</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>1000</v>
       </c>
-      <c r="L19" s="2">
-        <v>150</v>
-      </c>
       <c r="M19" s="2">
         <v>150</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="2">
+        <v>150</v>
+      </c>
+      <c r="O19" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="O19" s="2">
-        <v>3</v>
-      </c>
       <c r="P19" s="2">
         <v>3</v>
       </c>
-      <c r="Q19" s="2" t="s">
-        <v>0</v>
+      <c r="Q19" s="2">
+        <v>3</v>
       </c>
       <c r="R19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U19" s="2">
+      <c r="T19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -1960,722 +2110,755 @@
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="2">
         <v>400</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>60</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>120</v>
       </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
         <v>2200</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>1000</v>
       </c>
-      <c r="L20" s="2">
-        <v>150</v>
-      </c>
       <c r="M20" s="2">
         <v>150</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N20" s="2">
+        <v>150</v>
+      </c>
+      <c r="O20" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="O20" s="2">
-        <v>3</v>
-      </c>
       <c r="P20" s="2">
         <v>3</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>0</v>
+      <c r="Q20" s="2">
+        <v>3</v>
       </c>
       <c r="R20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="U20" s="2">
+      <c r="T20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2">
         <v>23</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="2">
         <v>400</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>60</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>120</v>
       </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
         <v>1800</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>1000</v>
       </c>
-      <c r="L21" s="2">
-        <v>150</v>
-      </c>
       <c r="M21" s="2">
         <v>150</v>
       </c>
-      <c r="N21" s="1">
-        <f t="shared" ref="N21" si="1">J21/100</f>
+      <c r="N21" s="2">
+        <v>150</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" ref="O21" si="1">K21/100</f>
         <v>18</v>
       </c>
-      <c r="O21" s="2">
-        <v>3</v>
-      </c>
       <c r="P21" s="2">
         <v>3</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>0</v>
+      <c r="Q21" s="2">
+        <v>3</v>
       </c>
       <c r="R21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="U21" s="2">
+      <c r="T21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V21" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2">
         <v>28</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="2">
         <v>400</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>60</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>120</v>
       </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1">
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
         <v>1800</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>1000</v>
       </c>
-      <c r="L22" s="2">
-        <v>150</v>
-      </c>
       <c r="M22" s="2">
         <v>150</v>
       </c>
-      <c r="N22" s="1">
-        <f t="shared" ref="N22" si="2">J22/100</f>
+      <c r="N22" s="2">
+        <v>150</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" ref="O22" si="2">K22/100</f>
         <v>18</v>
       </c>
-      <c r="O22" s="2">
-        <v>3</v>
-      </c>
       <c r="P22" s="2">
         <v>3</v>
       </c>
-      <c r="Q22" s="2" t="s">
-        <v>0</v>
+      <c r="Q22" s="2">
+        <v>3</v>
       </c>
       <c r="R22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="U22" s="2">
+      <c r="T22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V22" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2">
         <v>21</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="2">
         <v>400</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>60</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>120</v>
       </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
         <v>1800</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>1000</v>
       </c>
-      <c r="L23" s="2">
-        <v>150</v>
-      </c>
       <c r="M23" s="2">
         <v>150</v>
       </c>
-      <c r="N23" s="1">
-        <f t="shared" ref="N23" si="3">J23/100</f>
+      <c r="N23" s="2">
+        <v>150</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" ref="O23" si="3">K23/100</f>
         <v>18</v>
       </c>
-      <c r="O23" s="2">
-        <v>3</v>
-      </c>
       <c r="P23" s="2">
         <v>3</v>
       </c>
-      <c r="Q23" s="2" t="s">
-        <v>0</v>
+      <c r="Q23" s="2">
+        <v>3</v>
       </c>
       <c r="R23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="U23" s="2">
+      <c r="T23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="2">
         <v>17</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="2">
         <v>400</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>60</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>120</v>
       </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
         <v>1800</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>1000</v>
       </c>
-      <c r="L24" s="2">
-        <v>150</v>
-      </c>
       <c r="M24" s="2">
         <v>150</v>
       </c>
-      <c r="N24" s="1">
-        <f t="shared" ref="N24" si="4">J24/100</f>
+      <c r="N24" s="2">
+        <v>150</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" ref="O24" si="4">K24/100</f>
         <v>18</v>
       </c>
-      <c r="O24" s="2">
-        <v>3</v>
-      </c>
       <c r="P24" s="2">
         <v>3</v>
       </c>
-      <c r="Q24" s="2" t="s">
-        <v>0</v>
+      <c r="Q24" s="2">
+        <v>3</v>
       </c>
       <c r="R24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="U24" s="2">
+      <c r="T24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V24" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2">
         <v>26</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="2">
         <v>400</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>60</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>120</v>
       </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
         <v>1800</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>1000</v>
       </c>
-      <c r="L25" s="2">
-        <v>150</v>
-      </c>
       <c r="M25" s="2">
         <v>150</v>
       </c>
-      <c r="N25" s="1">
-        <f t="shared" ref="N25" si="5">J25/100</f>
+      <c r="N25" s="2">
+        <v>150</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" ref="O25" si="5">K25/100</f>
         <v>18</v>
       </c>
-      <c r="O25" s="2">
-        <v>3</v>
-      </c>
       <c r="P25" s="2">
         <v>3</v>
       </c>
-      <c r="Q25" s="2" t="s">
-        <v>0</v>
+      <c r="Q25" s="2">
+        <v>3</v>
       </c>
       <c r="R25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U25" s="2">
+      <c r="T25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="V25" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="2">
         <v>19</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="2">
         <v>400</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>60</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>120</v>
       </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
         <v>1800</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>1000</v>
       </c>
-      <c r="L26" s="2">
-        <v>150</v>
-      </c>
       <c r="M26" s="2">
         <v>150</v>
       </c>
-      <c r="N26" s="1">
-        <f t="shared" ref="N26" si="6">J26/100</f>
+      <c r="N26" s="2">
+        <v>150</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" ref="O26" si="6">K26/100</f>
         <v>18</v>
       </c>
-      <c r="O26" s="2">
-        <v>3</v>
-      </c>
       <c r="P26" s="2">
         <v>3</v>
       </c>
-      <c r="Q26" s="2" t="s">
-        <v>0</v>
+      <c r="Q26" s="2">
+        <v>3</v>
       </c>
       <c r="R26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="U26" s="2">
+      <c r="T26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="V26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2">
         <v>16</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="2">
         <v>400</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>60</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>120</v>
       </c>
-      <c r="I27" s="2">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
         <v>1800</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>1000</v>
       </c>
-      <c r="L27" s="2">
-        <v>150</v>
-      </c>
       <c r="M27" s="2">
         <v>150</v>
       </c>
-      <c r="N27" s="1">
-        <f t="shared" ref="N27:N28" si="7">J27/100</f>
+      <c r="N27" s="2">
+        <v>150</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" ref="O27:O28" si="7">K27/100</f>
         <v>18</v>
       </c>
-      <c r="O27" s="2">
-        <v>3</v>
-      </c>
       <c r="P27" s="2">
         <v>3</v>
       </c>
-      <c r="Q27" s="2" t="s">
-        <v>0</v>
+      <c r="Q27" s="2">
+        <v>3</v>
       </c>
       <c r="R27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="U27" s="2">
+      <c r="T27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="V27" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2">
         <v>20</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" s="2">
         <v>400</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>60</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>120</v>
       </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
         <v>1800</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>1000</v>
       </c>
-      <c r="L28" s="2">
-        <v>150</v>
-      </c>
       <c r="M28" s="2">
         <v>150</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N28" s="2">
+        <v>150</v>
+      </c>
+      <c r="O28" s="1">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="O28" s="2">
-        <v>3</v>
-      </c>
       <c r="P28" s="2">
         <v>3</v>
       </c>
-      <c r="Q28" s="2" t="s">
-        <v>0</v>
+      <c r="Q28" s="2">
+        <v>3</v>
       </c>
       <c r="R28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="U28" s="2">
+      <c r="T28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V28" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="2">
         <v>18</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="2">
         <v>400</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>60</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>120</v>
       </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
         <v>1800</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>1000</v>
       </c>
-      <c r="L29" s="2">
-        <v>150</v>
-      </c>
       <c r="M29" s="2">
         <v>150</v>
       </c>
-      <c r="N29" s="1">
-        <f t="shared" ref="N29:N31" si="8">J29/100</f>
+      <c r="N29" s="2">
+        <v>150</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" ref="O29:O31" si="8">K29/100</f>
         <v>18</v>
       </c>
-      <c r="O29" s="2">
-        <v>3</v>
-      </c>
       <c r="P29" s="2">
         <v>3</v>
       </c>
-      <c r="Q29" s="2" t="s">
-        <v>0</v>
+      <c r="Q29" s="2">
+        <v>3</v>
       </c>
       <c r="R29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="U29" s="2">
+      <c r="T29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="V29" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="2">
         <v>30</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="2">
         <v>400</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>60</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>120</v>
       </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
         <v>1800</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
         <v>1000</v>
       </c>
-      <c r="L30" s="2">
-        <v>150</v>
-      </c>
       <c r="M30" s="2">
         <v>150</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N30" s="2">
+        <v>150</v>
+      </c>
+      <c r="O30" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="O30" s="2">
-        <v>3</v>
-      </c>
       <c r="P30" s="2">
         <v>3</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>0</v>
+      <c r="Q30" s="2">
+        <v>3</v>
       </c>
       <c r="R30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="U30" s="2">
+      <c r="T30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V30" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>39</v>
@@ -2686,53 +2869,56 @@
       <c r="E31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="2">
         <v>400</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>60</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>120</v>
       </c>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
         <v>1800</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>1000</v>
       </c>
-      <c r="L31" s="2">
-        <v>150</v>
-      </c>
       <c r="M31" s="2">
         <v>150</v>
       </c>
-      <c r="N31" s="1">
+      <c r="N31" s="2">
+        <v>150</v>
+      </c>
+      <c r="O31" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="O31" s="2">
-        <v>3</v>
-      </c>
       <c r="P31" s="2">
         <v>3</v>
       </c>
-      <c r="Q31" s="2" t="s">
-        <v>0</v>
+      <c r="Q31" s="2">
+        <v>3</v>
       </c>
       <c r="R31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="U31" s="2">
+      <c r="T31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="V31" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created separate files for B1
To deal with CRM8
</commit_message>
<xml_diff>
--- a/airica/data/Aug_20_Wadden_sea_B1_AIRICA.xlsx
+++ b/airica/data/Aug_20_Wadden_sea_B1_AIRICA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/lab-work/airica/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{2ADD0B49-2137-472B-837C-A2FF8AF723D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A38AABAD-4399-435F-9E1D-3FC117ACB8FE}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="8_{2ADD0B49-2137-472B-837C-A2FF8AF723D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD5B91C7-E363-44C8-B8F8-E6F15747E2C7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D1C24D6-B482-4633-80E7-FE6A1A2CCD8F}"/>
   </bookViews>
@@ -739,7 +739,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W17" sqref="W17"/>
+      <selection pane="bottomLeft" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>